<commit_message>
91 exceles, a revisar
</commit_message>
<xml_diff>
--- a/public/u_excel/1.LM.2.xlsx
+++ b/public/u_excel/1.LM.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zizek\Desktop\Repositorio\dev-bomberos\public\u_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B987140-1AE6-4442-AFD4-B81466957849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0941757C-AC6C-48F4-AF23-92C97A8DDFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Nombre</t>
   </si>
@@ -46,22 +46,6 @@
     <t>San Francisco Tres Jacales</t>
   </si>
   <si>
-    <r>
-      <t>Altitud</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>c/</t>
-    </r>
-  </si>
-  <si>
     <t>106°29'06.067" W</t>
   </si>
   <si>
@@ -156,37 +140,6 @@
   </si>
   <si>
     <t>31°28'25''</t>
-  </si>
-  <si>
-    <r>
-      <t>Altitud</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ciudad Juárez </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>/d</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Población </t>
@@ -323,6 +276,37 @@
       <t xml:space="preserve"> Cabecera municipal</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>Altitud</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(c)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ciudad Juárez </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(d)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -705,7 +689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -821,15 +805,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -898,46 +873,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -946,71 +882,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1059,89 +931,65 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="34" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="34" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1488,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1502,373 +1350,373 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19">
         <v>2010</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="22" t="s">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="4">
+        <v>1137</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1321004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="23">
-        <v>1137</v>
-      </c>
-      <c r="E3" s="23">
-        <v>1321004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="24" t="s">
+      <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="D4" s="6">
+        <v>1113</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="25">
-        <v>1113</v>
-      </c>
-      <c r="E4" s="25">
-        <v>3483</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="D5" s="4">
+        <v>1120</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="23">
-        <v>1120</v>
-      </c>
-      <c r="E5" s="23">
-        <v>2169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="24" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="D6" s="6">
+        <v>1263</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="25">
-        <v>1263</v>
-      </c>
-      <c r="E6" s="25">
-        <v>1474</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="22" t="s">
+      <c r="C7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="D7" s="4">
+        <v>1121</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="23">
-        <v>1121</v>
-      </c>
-      <c r="E7" s="23">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="24" t="s">
+      <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="D8" s="6">
+        <v>1100</v>
+      </c>
+      <c r="E8" s="5">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="25">
-        <v>1100</v>
-      </c>
-      <c r="E8" s="24">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="22" t="s">
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="D9" s="4">
+        <v>1117</v>
+      </c>
+      <c r="E9" s="3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="23">
-        <v>1117</v>
-      </c>
-      <c r="E9" s="22">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="24" t="s">
+      <c r="C10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="25">
+      <c r="D10" s="6">
         <v>1110</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="5">
         <v>236</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="20">
         <v>2020</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" ht="31.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1131</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1501551</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1116</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1129</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="6">
+        <v>1262</v>
+      </c>
+      <c r="E16" s="6">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1120</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1104</v>
+      </c>
+      <c r="E18" s="6">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1101</v>
+      </c>
+      <c r="E19" s="4">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1104</v>
+      </c>
+      <c r="E20" s="5">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="23">
-        <v>1131</v>
-      </c>
-      <c r="E13" s="23">
-        <v>1501551</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="25">
-        <v>1116</v>
-      </c>
-      <c r="E14" s="25">
-        <v>3383</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="23">
-        <v>1129</v>
-      </c>
-      <c r="E15" s="23">
-        <v>2065</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="25">
-        <v>1262</v>
-      </c>
-      <c r="E16" s="25">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="23">
-        <v>1120</v>
-      </c>
-      <c r="E17" s="23">
-        <v>1373</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="25">
-        <v>1104</v>
-      </c>
-      <c r="E18" s="25">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="23">
-        <v>1101</v>
-      </c>
-      <c r="E19" s="23">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="25">
-        <v>1104</v>
-      </c>
-      <c r="E20" s="24">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29"/>

</xml_diff>